<commit_message>
Added a new question to document.
</commit_message>
<xml_diff>
--- a/MySQL - w3schools.xlsx
+++ b/MySQL - w3schools.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25200" windowHeight="12075"/>
+    <workbookView windowWidth="25200" windowHeight="12135"/>
   </bookViews>
   <sheets>
     <sheet name="MySQL" sheetId="1" r:id="rId1"/>
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Now</t>
   </si>
@@ -203,6 +203,9 @@
   </si>
   <si>
     <t>How do you delete a table?</t>
+  </si>
+  <si>
+    <t>How do you delete all data in a table?</t>
   </si>
   <si>
     <t>How do you add/delete a column?</t>
@@ -298,11 +301,11 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
-    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
     <numFmt numFmtId="42" formatCode="_-&quot;£&quot;* #,##0_-;\-&quot;£&quot;* #,##0_-;_-&quot;£&quot;* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
+    <numFmt numFmtId="44" formatCode="_-&quot;£&quot;* #,##0.00_-;\-&quot;£&quot;* #,##0.00_-;_-&quot;£&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="23">
+  <fonts count="24">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -327,6 +330,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="9"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -334,14 +344,28 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -355,51 +379,18 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <i/>
-      <sz val="11"/>
-      <color rgb="FF7F7F7F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -411,16 +402,63 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
       <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -435,49 +473,21 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="0"/>
+      <i/>
+      <sz val="11"/>
+      <color rgb="FF7F7F7F"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF9C6500"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
   </fonts>
-  <fills count="34">
+  <fills count="33">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -492,25 +502,163 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,157 +670,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
+        <fgColor theme="9" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -710,11 +714,35 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FF7F7F7F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF7F7F7F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF7F7F7F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF7F7F7F"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom style="medium">
         <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -749,26 +777,13 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FF7F7F7F"/>
-      </left>
-      <right style="thin">
-        <color rgb="FF7F7F7F"/>
-      </right>
-      <top style="thin">
-        <color rgb="FF7F7F7F"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FF7F7F7F"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -790,17 +805,6 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="double">
         <color rgb="FFFF8001"/>
@@ -812,152 +816,152 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="11" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="30" borderId="9" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="4" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="16" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -976,7 +980,10 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1298,10 +1305,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:D92"/>
+  <dimension ref="A1:D93"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D11" sqref="D11"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="D64" sqref="D64"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="15" outlineLevelCol="3"/>
@@ -1361,32 +1368,38 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="4:4">
+    <row r="11" spans="1:4">
+      <c r="A11" s="6"/>
       <c r="D11" s="2" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="4:4">
+    <row r="12" spans="1:4">
+      <c r="A12" s="3"/>
       <c r="D12" s="2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="4:4">
+    <row r="13" spans="1:4">
+      <c r="A13" s="3"/>
       <c r="D13" s="2" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="4:4">
+    <row r="14" spans="1:4">
+      <c r="A14" s="3"/>
       <c r="D14" s="2" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="15" spans="4:4">
+    <row r="15" spans="1:4">
+      <c r="A15" s="3"/>
       <c r="D15" s="2" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="16" spans="4:4">
+    <row r="16" spans="1:4">
+      <c r="A16" s="3"/>
       <c r="D16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1761,14 +1774,19 @@
         <v>88</v>
       </c>
     </row>
-    <row r="91" customHeight="1" spans="4:4">
-      <c r="D91" s="6" t="s">
+    <row r="91" spans="4:4">
+      <c r="D91" s="2" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="92" spans="4:4">
-      <c r="D92" s="2" t="s">
+    <row r="92" customHeight="1" spans="4:4">
+      <c r="D92" s="7" t="s">
         <v>90</v>
+      </c>
+    </row>
+    <row r="93" spans="4:4">
+      <c r="D93" s="2" t="s">
+        <v>91</v>
       </c>
     </row>
   </sheetData>

</xml_diff>